<commit_message>
final push for now, may be refactored later
</commit_message>
<xml_diff>
--- a/data/metadata2.xlsx
+++ b/data/metadata2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,306 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>BR50041</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BR50042</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BR50045</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BR50047</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BR50050</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>